<commit_message>
added prideti, susije doc
</commit_message>
<xml_diff>
--- a/Task1(v4)/results.xlsx
+++ b/Task1(v4)/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" xr2:uid="{B38044DC-E526-4749-995C-5A23170718C6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" xr2:uid="{D379EB45-A4C8-437A-9ACD-90FC6141511E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B0DC7E-BC09-4456-9A83-5699047CD400}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658ED75B-4196-464B-BC12-9D927689F5FB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>